<commit_message>
update vibrio colony counts
</commit_message>
<xml_diff>
--- a/OysterHatcheryMicrobiome_orderdata.xlsx
+++ b/OysterHatcheryMicrobiome_orderdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjste\Documents\URI\Research\RWU Hatchery Trials\16S\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1CF722-65A7-4A5A-80E4-9D9273739A59}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB73BF91-EE56-4A4F-A370-F4D5DDAF8A32}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="water_trans" sheetId="2" r:id="rId1"/>
@@ -21,13 +21,14 @@
     <sheet name="trial2_trans" sheetId="5" r:id="rId6"/>
     <sheet name="trial2_meta" sheetId="7" r:id="rId7"/>
     <sheet name="trial3_all" sheetId="9" r:id="rId8"/>
+    <sheet name="VibrioCounts" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="337">
   <si>
     <t>taxa</t>
   </si>
@@ -1030,6 +1031,15 @@
   <si>
     <t>12_outflow_Outflow</t>
   </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>Replicate</t>
+  </si>
+  <si>
+    <t>VibrioColonyCounts</t>
+  </si>
 </sst>
 </file>
 
@@ -1512,9 +1522,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -86082,8 +86095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB777A6C-0E65-41D4-8280-FE8D035B085E}">
   <dimension ref="A1:AC25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:AE63"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -88319,4 +88332,877 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47560CCF-76C9-463C-8238-F4D005FA3B0F}">
+  <dimension ref="A1:G37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N41" sqref="N41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" t="s">
+        <v>335</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1666.6666666666667</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1333.3333333333333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1666.6666666666667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" t="s">
+        <v>274</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>202</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>177.77777777777777</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>202</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7" s="2">
+        <v>177.77777777777777</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>203</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9" t="s">
+        <v>274</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" s="2">
+        <v>488.88888888888891</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>166</v>
+      </c>
+      <c r="B10" t="s">
+        <v>274</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>203</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10" s="2">
+        <v>711.11111111111109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11" t="s">
+        <v>274</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>202</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>168</v>
+      </c>
+      <c r="B12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>202</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>169</v>
+      </c>
+      <c r="B13" t="s">
+        <v>274</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>202</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13" s="2">
+        <v>88.888888888888886</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>204</v>
+      </c>
+      <c r="B14" t="s">
+        <v>272</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>203</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>5333.333333333333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>205</v>
+      </c>
+      <c r="B15" t="s">
+        <v>272</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>203</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>4888.8888888888896</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>206</v>
+      </c>
+      <c r="B16" t="s">
+        <v>272</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
+        <v>203</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="G16" s="1">
+        <v>7555.5555555555557</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>207</v>
+      </c>
+      <c r="B17" t="s">
+        <v>272</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>202</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1333.3333333333333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>208</v>
+      </c>
+      <c r="B18" t="s">
+        <v>272</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>202</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>209</v>
+      </c>
+      <c r="B19" t="s">
+        <v>272</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
+        <v>202</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>210</v>
+      </c>
+      <c r="B20" t="s">
+        <v>272</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>203</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>155.55555555555554</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>211</v>
+      </c>
+      <c r="B21" t="s">
+        <v>272</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>203</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1166.6666666666665</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>212</v>
+      </c>
+      <c r="B22" t="s">
+        <v>272</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>203</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22" s="1">
+        <v>122.22222222222221</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>213</v>
+      </c>
+      <c r="B23" t="s">
+        <v>272</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>202</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1">
+        <v>44.444444444444443</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>214</v>
+      </c>
+      <c r="B24" t="s">
+        <v>272</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>202</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1">
+        <v>211.11111111111111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>215</v>
+      </c>
+      <c r="B25" t="s">
+        <v>272</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>202</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+      <c r="G25" s="1">
+        <v>155.55555555555554</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>216</v>
+      </c>
+      <c r="B26" t="s">
+        <v>273</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>12</v>
+      </c>
+      <c r="E26" t="s">
+        <v>203</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26" s="2">
+        <v>19111.111111111109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>217</v>
+      </c>
+      <c r="B27" t="s">
+        <v>273</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>12</v>
+      </c>
+      <c r="E27" t="s">
+        <v>203</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27" s="2">
+        <v>2333.333333333333</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>218</v>
+      </c>
+      <c r="B28" t="s">
+        <v>273</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s">
+        <v>203</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+      <c r="G28" s="2">
+        <v>13555.555555555555</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>219</v>
+      </c>
+      <c r="B29" t="s">
+        <v>273</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>12</v>
+      </c>
+      <c r="E29" t="s">
+        <v>202</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>220</v>
+      </c>
+      <c r="B30" t="s">
+        <v>273</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
+        <v>202</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30" s="2">
+        <v>4666.666666666667</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>221</v>
+      </c>
+      <c r="B31" t="s">
+        <v>273</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>12</v>
+      </c>
+      <c r="E31" t="s">
+        <v>202</v>
+      </c>
+      <c r="F31">
+        <v>3</v>
+      </c>
+      <c r="G31" s="2">
+        <v>2222.2222222222217</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>222</v>
+      </c>
+      <c r="B32" t="s">
+        <v>273</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
+      </c>
+      <c r="E32" t="s">
+        <v>203</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>223</v>
+      </c>
+      <c r="B33" t="s">
+        <v>273</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>203</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33" s="2">
+        <v>9666.6666666666661</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>224</v>
+      </c>
+      <c r="B34" t="s">
+        <v>273</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="E34" t="s">
+        <v>203</v>
+      </c>
+      <c r="F34">
+        <v>3</v>
+      </c>
+      <c r="G34" s="2">
+        <v>511.11111111111114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>225</v>
+      </c>
+      <c r="B35" t="s">
+        <v>273</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>202</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35" s="2">
+        <v>122.22222222222221</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>226</v>
+      </c>
+      <c r="B36" t="s">
+        <v>273</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
+      <c r="E36" t="s">
+        <v>202</v>
+      </c>
+      <c r="F36">
+        <v>2</v>
+      </c>
+      <c r="G36" s="2">
+        <v>311.11111111111109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>227</v>
+      </c>
+      <c r="B37" t="s">
+        <v>273</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
+      <c r="E37" t="s">
+        <v>202</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+      <c r="G37" s="2">
+        <v>88.8888888888889</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>